<commit_message>
Extend the sensor_table and the example one by the three columns "Sensitivity Error", "Linearity Error", "Hysteresis Error" and rename the bias and offset column
</commit_message>
<xml_diff>
--- a/sensor_table.xlsx
+++ b/sensor_table.xlsx
@@ -14,10 +14,10 @@
     <sheet name="Temperatur" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Druck!$A$1:$X$134</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$V$19</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$V$25</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$V$21</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Druck!$A$1:$AA$68</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$Y$13</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$Y$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$Y$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="27">
   <si>
     <t xml:space="preserve">uuid</t>
   </si>
@@ -58,10 +58,19 @@
     <t xml:space="preserve">Ausgabebereich Einheit</t>
   </si>
   <si>
-    <t xml:space="preserve">Kennlinie Steigung</t>
+    <t xml:space="preserve">Kennlinie Steigung _ Sensitivity</t>
   </si>
   <si>
-    <t xml:space="preserve">Kennlinie Offset</t>
+    <t xml:space="preserve">Kennlinie Offset _ Bias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensitivity Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linearity Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hysteresis Error</t>
   </si>
   <si>
     <t xml:space="preserve">Messprinzip</t>
@@ -469,17 +478,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X183"/>
+  <dimension ref="A1:AA203"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -489,9 +498,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="27.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="14.86"/>
@@ -532,10 +541,10 @@
       <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -547,7 +556,7 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
@@ -570,6 +579,15 @@
       </c>
       <c r="X1" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -584,12 +602,12 @@
       <c r="I2" s="3"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="Q2" s="4"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -597,237 +615,339 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="7"/>
       <c r="H3" s="8"/>
-      <c r="P3" s="7"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="S3" s="7"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
     </row>
     <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="7"/>
       <c r="H4" s="8"/>
-      <c r="P4" s="7"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="S4" s="7"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
     </row>
     <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="7"/>
       <c r="H5" s="8"/>
-      <c r="P5" s="7"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="S5" s="7"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
     </row>
     <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7"/>
       <c r="H6" s="8"/>
-      <c r="P6" s="7"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
+      <c r="S6" s="7"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
     </row>
     <row r="7" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="7"/>
       <c r="H7" s="8"/>
-      <c r="P7" s="7"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="S7" s="7"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
     </row>
     <row r="8" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="7"/>
       <c r="H8" s="8"/>
-      <c r="P8" s="7"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="S8" s="7"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
     </row>
     <row r="9" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="7"/>
       <c r="H9" s="8"/>
-      <c r="P9" s="7"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
+      <c r="S9" s="7"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
     </row>
     <row r="10" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="7"/>
       <c r="H10" s="8"/>
-      <c r="P10" s="7"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="N10" s="0"/>
+      <c r="S10" s="7"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
     </row>
     <row r="11" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="7"/>
       <c r="H11" s="8"/>
-      <c r="P11" s="7"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
+      <c r="S11" s="7"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
     </row>
     <row r="12" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="7"/>
       <c r="H12" s="8"/>
-      <c r="P12" s="7"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
+      <c r="N12" s="0"/>
+      <c r="S12" s="7"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
     </row>
     <row r="13" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="7"/>
       <c r="H13" s="8"/>
-      <c r="P13" s="7"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="N13" s="0"/>
+      <c r="S13" s="7"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
     </row>
     <row r="14" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="7"/>
       <c r="H14" s="8"/>
-      <c r="P14" s="7"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
+      <c r="N14" s="0"/>
+      <c r="S14" s="7"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
     </row>
     <row r="15" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="7"/>
       <c r="H15" s="8"/>
-      <c r="P15" s="7"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
+      <c r="L15" s="0"/>
+      <c r="M15" s="0"/>
+      <c r="N15" s="0"/>
+      <c r="S15" s="7"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
     </row>
     <row r="16" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7"/>
       <c r="H16" s="8"/>
-      <c r="P16" s="7"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
+      <c r="L16" s="0"/>
+      <c r="M16" s="0"/>
+      <c r="N16" s="0"/>
+      <c r="S16" s="7"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
     </row>
     <row r="17" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="7"/>
       <c r="H17" s="8"/>
-      <c r="P17" s="7"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
+      <c r="L17" s="0"/>
+      <c r="M17" s="0"/>
+      <c r="N17" s="0"/>
+      <c r="S17" s="7"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
     </row>
     <row r="18" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="7"/>
       <c r="H18" s="8"/>
-      <c r="P18" s="7"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
+      <c r="L18" s="0"/>
+      <c r="M18" s="0"/>
+      <c r="N18" s="0"/>
+      <c r="S18" s="7"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
     </row>
     <row r="19" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="7"/>
       <c r="H19" s="8"/>
-      <c r="P19" s="7"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
+      <c r="L19" s="0"/>
+      <c r="M19" s="0"/>
+      <c r="N19" s="0"/>
+      <c r="S19" s="7"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
     </row>
     <row r="20" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7"/>
       <c r="H20" s="8"/>
-      <c r="P20" s="7"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
+      <c r="L20" s="0"/>
+      <c r="M20" s="0"/>
+      <c r="N20" s="0"/>
+      <c r="S20" s="7"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
     </row>
     <row r="21" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="7"/>
       <c r="H21" s="8"/>
-      <c r="P21" s="7"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
+      <c r="L21" s="0"/>
+      <c r="M21" s="0"/>
+      <c r="N21" s="0"/>
+      <c r="S21" s="7"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
     </row>
     <row r="22" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7"/>
       <c r="H22" s="8"/>
-      <c r="P22" s="7"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
+      <c r="L22" s="0"/>
+      <c r="M22" s="0"/>
+      <c r="N22" s="0"/>
+      <c r="S22" s="7"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
     </row>
     <row r="23" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="7"/>
       <c r="H23" s="8"/>
-      <c r="P23" s="7"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
+      <c r="L23" s="0"/>
+      <c r="M23" s="0"/>
+      <c r="N23" s="0"/>
+      <c r="S23" s="7"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
     </row>
     <row r="24" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="7"/>
       <c r="H24" s="8"/>
-      <c r="P24" s="7"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
+      <c r="L24" s="0"/>
+      <c r="M24" s="0"/>
+      <c r="N24" s="0"/>
+      <c r="S24" s="7"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
     </row>
     <row r="25" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="7"/>
       <c r="H25" s="8"/>
-      <c r="P25" s="7"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
+      <c r="L25" s="0"/>
+      <c r="M25" s="0"/>
+      <c r="N25" s="0"/>
+      <c r="S25" s="7"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
     </row>
     <row r="26" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="7"/>
       <c r="H26" s="8"/>
-      <c r="P26" s="7"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
+      <c r="L26" s="0"/>
+      <c r="M26" s="0"/>
+      <c r="N26" s="0"/>
+      <c r="S26" s="7"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
     </row>
     <row r="27" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="7"/>
       <c r="H27" s="8"/>
-      <c r="P27" s="7"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
+      <c r="L27" s="0"/>
+      <c r="M27" s="0"/>
+      <c r="N27" s="0"/>
+      <c r="S27" s="7"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
     </row>
     <row r="28" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="7"/>
       <c r="H28" s="8"/>
-      <c r="P28" s="7"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
+      <c r="L28" s="0"/>
+      <c r="M28" s="0"/>
+      <c r="N28" s="0"/>
+      <c r="S28" s="7"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
     </row>
     <row r="29" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="7"/>
       <c r="H29" s="8"/>
-      <c r="P29" s="7"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
+      <c r="L29" s="0"/>
+      <c r="M29" s="0"/>
+      <c r="N29" s="0"/>
+      <c r="S29" s="7"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
     </row>
     <row r="30" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="7"/>
       <c r="H30" s="8"/>
-      <c r="P30" s="7"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
+      <c r="L30" s="0"/>
+      <c r="M30" s="0"/>
+      <c r="N30" s="0"/>
+      <c r="S30" s="7"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
     </row>
     <row r="31" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="7"/>
       <c r="H31" s="8"/>
-      <c r="P31" s="7"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
+      <c r="L31" s="0"/>
+      <c r="M31" s="0"/>
+      <c r="N31" s="0"/>
+      <c r="S31" s="7"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
     </row>
     <row r="32" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="7"/>
       <c r="H32" s="8"/>
-      <c r="P32" s="7"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
+      <c r="L32" s="0"/>
+      <c r="M32" s="0"/>
+      <c r="N32" s="0"/>
+      <c r="S32" s="7"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
     </row>
     <row r="33" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="7"/>
       <c r="H33" s="8"/>
-      <c r="P33" s="7"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
+      <c r="L33" s="0"/>
+      <c r="M33" s="0"/>
+      <c r="N33" s="0"/>
+      <c r="S33" s="7"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
     </row>
     <row r="34" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="7"/>
       <c r="H34" s="8"/>
-      <c r="P34" s="7"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
+      <c r="L34" s="0"/>
+      <c r="M34" s="0"/>
+      <c r="N34" s="0"/>
+      <c r="S34" s="7"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
     </row>
     <row r="35" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="7"/>
       <c r="H35" s="8"/>
-      <c r="P35" s="7"/>
-      <c r="S35" s="8"/>
+      <c r="L35" s="0"/>
+      <c r="M35" s="0"/>
+      <c r="N35" s="0"/>
+      <c r="S35" s="7"/>
+      <c r="V35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="7"/>
@@ -836,11 +956,12 @@
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
+      <c r="L36" s="0"/>
       <c r="O36" s="8"/>
-      <c r="P36" s="1"/>
-      <c r="S36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="1"/>
+      <c r="V36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="7"/>
@@ -849,11 +970,12 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
+      <c r="L37" s="0"/>
       <c r="O37" s="8"/>
-      <c r="P37" s="1"/>
-      <c r="S37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="1"/>
+      <c r="V37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="7"/>
@@ -862,11 +984,12 @@
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
+      <c r="L38" s="0"/>
       <c r="O38" s="8"/>
-      <c r="P38" s="1"/>
-      <c r="S38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="1"/>
+      <c r="V38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="7"/>
@@ -875,11 +998,12 @@
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
+      <c r="L39" s="0"/>
       <c r="O39" s="8"/>
-      <c r="P39" s="1"/>
-      <c r="S39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="1"/>
+      <c r="V39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="7"/>
@@ -888,11 +1012,12 @@
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
+      <c r="L40" s="0"/>
       <c r="O40" s="8"/>
-      <c r="P40" s="1"/>
-      <c r="S40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="1"/>
+      <c r="V40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="7"/>
@@ -901,11 +1026,12 @@
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
+      <c r="L41" s="0"/>
       <c r="O41" s="8"/>
-      <c r="P41" s="1"/>
-      <c r="S41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="1"/>
+      <c r="V41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="7"/>
@@ -914,11 +1040,12 @@
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
+      <c r="L42" s="0"/>
       <c r="O42" s="8"/>
-      <c r="P42" s="1"/>
-      <c r="S42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="1"/>
+      <c r="V42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="7"/>
@@ -927,11 +1054,12 @@
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
+      <c r="L43" s="0"/>
       <c r="O43" s="8"/>
-      <c r="P43" s="1"/>
-      <c r="S43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="1"/>
+      <c r="V43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="7"/>
@@ -940,11 +1068,12 @@
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
+      <c r="L44" s="0"/>
       <c r="O44" s="8"/>
-      <c r="P44" s="1"/>
-      <c r="S44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="1"/>
+      <c r="V44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="7"/>
@@ -953,11 +1082,12 @@
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
+      <c r="L45" s="0"/>
       <c r="O45" s="8"/>
-      <c r="P45" s="1"/>
-      <c r="S45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="1"/>
+      <c r="V45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="7"/>
@@ -966,11 +1096,12 @@
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
+      <c r="L46" s="0"/>
       <c r="O46" s="8"/>
-      <c r="P46" s="1"/>
-      <c r="S46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="1"/>
+      <c r="V46" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="7"/>
@@ -979,11 +1110,12 @@
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
+      <c r="L47" s="0"/>
       <c r="O47" s="8"/>
-      <c r="P47" s="1"/>
-      <c r="S47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="1"/>
+      <c r="V47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="7"/>
@@ -992,11 +1124,12 @@
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
+      <c r="L48" s="0"/>
       <c r="O48" s="8"/>
-      <c r="P48" s="1"/>
-      <c r="S48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="1"/>
+      <c r="V48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="7"/>
@@ -1005,11 +1138,12 @@
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
+      <c r="L49" s="0"/>
       <c r="O49" s="8"/>
-      <c r="P49" s="1"/>
-      <c r="S49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="1"/>
+      <c r="V49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="7"/>
@@ -1018,11 +1152,12 @@
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
+      <c r="L50" s="0"/>
       <c r="O50" s="8"/>
-      <c r="P50" s="1"/>
-      <c r="S50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="R50" s="8"/>
+      <c r="S50" s="1"/>
+      <c r="V50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="7"/>
@@ -1031,11 +1166,12 @@
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
+      <c r="L51" s="0"/>
       <c r="O51" s="8"/>
-      <c r="P51" s="1"/>
-      <c r="S51" s="8"/>
+      <c r="P51" s="8"/>
+      <c r="R51" s="8"/>
+      <c r="S51" s="1"/>
+      <c r="V51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="7"/>
@@ -1044,10 +1180,12 @@
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
-      <c r="M52" s="8"/>
-      <c r="O52" s="8"/>
-      <c r="P52" s="1"/>
-      <c r="S52" s="8"/>
+      <c r="L52" s="0"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="8"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="1"/>
+      <c r="V52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="7"/>
@@ -1056,10 +1194,12 @@
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
-      <c r="M53" s="8"/>
-      <c r="O53" s="8"/>
-      <c r="P53" s="1"/>
-      <c r="S53" s="8"/>
+      <c r="L53" s="0"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="8"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="1"/>
+      <c r="V53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="7"/>
@@ -1068,11 +1208,12 @@
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
+      <c r="L54" s="0"/>
       <c r="O54" s="8"/>
-      <c r="P54" s="1"/>
-      <c r="S54" s="8"/>
+      <c r="P54" s="8"/>
+      <c r="R54" s="8"/>
+      <c r="S54" s="1"/>
+      <c r="V54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="7"/>
@@ -1081,11 +1222,12 @@
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
-      <c r="L55" s="8"/>
-      <c r="M55" s="8"/>
+      <c r="L55" s="0"/>
       <c r="O55" s="8"/>
-      <c r="P55" s="1"/>
-      <c r="S55" s="8"/>
+      <c r="P55" s="8"/>
+      <c r="R55" s="8"/>
+      <c r="S55" s="1"/>
+      <c r="V55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="7"/>
@@ -1094,11 +1236,12 @@
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
+      <c r="L56" s="0"/>
       <c r="O56" s="8"/>
-      <c r="P56" s="1"/>
-      <c r="S56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="1"/>
+      <c r="V56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="7"/>
@@ -1107,11 +1250,12 @@
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="8"/>
+      <c r="L57" s="0"/>
       <c r="O57" s="8"/>
-      <c r="P57" s="1"/>
-      <c r="S57" s="8"/>
+      <c r="P57" s="8"/>
+      <c r="R57" s="8"/>
+      <c r="S57" s="1"/>
+      <c r="V57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7"/>
@@ -1120,11 +1264,12 @@
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
-      <c r="L58" s="8"/>
-      <c r="M58" s="8"/>
+      <c r="L58" s="0"/>
       <c r="O58" s="8"/>
-      <c r="P58" s="1"/>
-      <c r="S58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="1"/>
+      <c r="V58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="7"/>
@@ -1133,11 +1278,12 @@
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
-      <c r="L59" s="8"/>
-      <c r="M59" s="8"/>
+      <c r="L59" s="0"/>
       <c r="O59" s="8"/>
-      <c r="P59" s="1"/>
-      <c r="S59" s="8"/>
+      <c r="P59" s="8"/>
+      <c r="R59" s="8"/>
+      <c r="S59" s="1"/>
+      <c r="V59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="7"/>
@@ -1146,11 +1292,12 @@
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
-      <c r="L60" s="8"/>
-      <c r="M60" s="8"/>
+      <c r="L60" s="0"/>
       <c r="O60" s="8"/>
-      <c r="P60" s="1"/>
-      <c r="S60" s="8"/>
+      <c r="P60" s="8"/>
+      <c r="R60" s="8"/>
+      <c r="S60" s="1"/>
+      <c r="V60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="7"/>
@@ -1159,11 +1306,12 @@
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
-      <c r="L61" s="8"/>
-      <c r="M61" s="8"/>
+      <c r="L61" s="0"/>
       <c r="O61" s="8"/>
-      <c r="P61" s="1"/>
-      <c r="S61" s="8"/>
+      <c r="P61" s="8"/>
+      <c r="R61" s="8"/>
+      <c r="S61" s="1"/>
+      <c r="V61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="7"/>
@@ -1172,11 +1320,12 @@
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
-      <c r="L62" s="8"/>
-      <c r="M62" s="8"/>
+      <c r="L62" s="0"/>
       <c r="O62" s="8"/>
-      <c r="P62" s="1"/>
-      <c r="S62" s="8"/>
+      <c r="P62" s="8"/>
+      <c r="R62" s="8"/>
+      <c r="S62" s="1"/>
+      <c r="V62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="7"/>
@@ -1185,11 +1334,12 @@
       <c r="I63" s="6"/>
       <c r="J63" s="6"/>
       <c r="K63" s="6"/>
-      <c r="L63" s="8"/>
-      <c r="M63" s="8"/>
+      <c r="L63" s="0"/>
       <c r="O63" s="8"/>
-      <c r="P63" s="1"/>
-      <c r="S63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="R63" s="8"/>
+      <c r="S63" s="1"/>
+      <c r="V63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="7"/>
@@ -1198,171 +1348,210 @@
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
-      <c r="L64" s="8"/>
-      <c r="M64" s="8"/>
+      <c r="L64" s="0"/>
       <c r="O64" s="8"/>
-      <c r="P64" s="1"/>
-      <c r="S64" s="8"/>
+      <c r="P64" s="8"/>
+      <c r="R64" s="8"/>
+      <c r="S64" s="1"/>
+      <c r="V64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9"/>
       <c r="B65" s="7"/>
       <c r="J65" s="6"/>
       <c r="K65" s="6"/>
-      <c r="M65" s="8"/>
-      <c r="O65" s="8"/>
+      <c r="L65" s="0"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="8"/>
+      <c r="R65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="7"/>
-      <c r="M66" s="8"/>
-      <c r="O66" s="8"/>
+      <c r="L66" s="0"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="8"/>
+      <c r="R66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="7"/>
       <c r="J67" s="6"/>
       <c r="K67" s="6"/>
-      <c r="M67" s="8"/>
-      <c r="O67" s="8"/>
+      <c r="L67" s="0"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="8"/>
+      <c r="R67" s="8"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="7"/>
-      <c r="M68" s="8"/>
-      <c r="O68" s="8"/>
+      <c r="L68" s="0"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="8"/>
+      <c r="R68" s="8"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="7"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
-      <c r="M69" s="8"/>
-      <c r="O69" s="8"/>
-      <c r="P69" s="1"/>
-      <c r="S69" s="8"/>
+      <c r="L69" s="0"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="8"/>
+      <c r="R69" s="8"/>
+      <c r="S69" s="1"/>
+      <c r="V69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7"/>
       <c r="J70" s="6"/>
       <c r="K70" s="6"/>
-      <c r="M70" s="8"/>
-      <c r="O70" s="8"/>
-      <c r="P70" s="1"/>
-      <c r="S70" s="8"/>
+      <c r="L70" s="0"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="8"/>
+      <c r="R70" s="8"/>
+      <c r="S70" s="1"/>
+      <c r="V70" s="8"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="7"/>
       <c r="J71" s="6"/>
       <c r="K71" s="6"/>
-      <c r="M71" s="8"/>
-      <c r="O71" s="8"/>
-      <c r="P71" s="1"/>
-      <c r="S71" s="8"/>
+      <c r="L71" s="0"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="8"/>
+      <c r="R71" s="8"/>
+      <c r="S71" s="1"/>
+      <c r="V71" s="8"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="7"/>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
-      <c r="M72" s="8"/>
-      <c r="O72" s="8"/>
-      <c r="P72" s="1"/>
-      <c r="S72" s="8"/>
+      <c r="L72" s="0"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="8"/>
+      <c r="R72" s="8"/>
+      <c r="S72" s="1"/>
+      <c r="V72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="7"/>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
-      <c r="M73" s="8"/>
-      <c r="O73" s="8"/>
-      <c r="P73" s="1"/>
-      <c r="S73" s="8"/>
+      <c r="L73" s="0"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="8"/>
+      <c r="R73" s="8"/>
+      <c r="S73" s="1"/>
+      <c r="V73" s="8"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="7"/>
       <c r="J74" s="6"/>
       <c r="K74" s="6"/>
-      <c r="M74" s="8"/>
-      <c r="O74" s="8"/>
-      <c r="P74" s="1"/>
-      <c r="S74" s="8"/>
+      <c r="L74" s="0"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="8"/>
+      <c r="R74" s="8"/>
+      <c r="S74" s="1"/>
+      <c r="V74" s="8"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="7"/>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
-      <c r="M75" s="8"/>
-      <c r="O75" s="8"/>
-      <c r="P75" s="1"/>
-      <c r="S75" s="8"/>
+      <c r="L75" s="0"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="8"/>
+      <c r="R75" s="8"/>
+      <c r="S75" s="1"/>
+      <c r="V75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="7"/>
       <c r="J76" s="6"/>
       <c r="K76" s="6"/>
-      <c r="M76" s="8"/>
-      <c r="O76" s="8"/>
-      <c r="P76" s="10"/>
-      <c r="S76" s="8"/>
+      <c r="L76" s="0"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="8"/>
+      <c r="R76" s="8"/>
+      <c r="S76" s="10"/>
+      <c r="V76" s="8"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="7"/>
       <c r="J77" s="6"/>
       <c r="K77" s="6"/>
-      <c r="M77" s="8"/>
-      <c r="O77" s="8"/>
-      <c r="P77" s="10"/>
-      <c r="S77" s="8"/>
+      <c r="L77" s="0"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="8"/>
+      <c r="R77" s="8"/>
+      <c r="S77" s="10"/>
+      <c r="V77" s="8"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="7"/>
       <c r="J78" s="6"/>
       <c r="K78" s="6"/>
-      <c r="M78" s="8"/>
-      <c r="O78" s="8"/>
-      <c r="P78" s="10"/>
-      <c r="S78" s="8"/>
+      <c r="L78" s="0"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="8"/>
+      <c r="R78" s="8"/>
+      <c r="S78" s="10"/>
+      <c r="V78" s="8"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="7"/>
       <c r="J79" s="6"/>
       <c r="K79" s="6"/>
-      <c r="M79" s="8"/>
-      <c r="O79" s="8"/>
-      <c r="P79" s="1"/>
-      <c r="S79" s="8"/>
+      <c r="L79" s="0"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="8"/>
+      <c r="R79" s="8"/>
+      <c r="S79" s="1"/>
+      <c r="V79" s="8"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="7"/>
       <c r="J80" s="6"/>
       <c r="K80" s="6"/>
-      <c r="M80" s="8"/>
-      <c r="O80" s="8"/>
-      <c r="P80" s="1"/>
-      <c r="S80" s="8"/>
+      <c r="L80" s="0"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="8"/>
+      <c r="R80" s="8"/>
+      <c r="S80" s="1"/>
+      <c r="V80" s="8"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="7"/>
       <c r="J81" s="6"/>
       <c r="K81" s="6"/>
-      <c r="M81" s="8"/>
-      <c r="O81" s="8"/>
-      <c r="P81" s="1"/>
-      <c r="S81" s="8"/>
+      <c r="L81" s="0"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="8"/>
+      <c r="R81" s="8"/>
+      <c r="S81" s="1"/>
+      <c r="V81" s="8"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="7"/>
       <c r="J82" s="6"/>
       <c r="K82" s="6"/>
-      <c r="M82" s="8"/>
-      <c r="O82" s="8"/>
-      <c r="P82" s="1"/>
-      <c r="S82" s="8"/>
+      <c r="L82" s="0"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="8"/>
+      <c r="R82" s="8"/>
+      <c r="S82" s="1"/>
+      <c r="V82" s="8"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="7"/>
       <c r="J83" s="6"/>
       <c r="K83" s="6"/>
-      <c r="M83" s="8"/>
-      <c r="O83" s="8"/>
-      <c r="P83" s="1"/>
-      <c r="S83" s="8"/>
+      <c r="L83" s="0"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="8"/>
+      <c r="R83" s="8"/>
+      <c r="S83" s="1"/>
+      <c r="V83" s="8"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L84" s="0"/>
@@ -1380,61 +1569,71 @@
       <c r="B88" s="7"/>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
-      <c r="M88" s="8"/>
-      <c r="O88" s="8"/>
-      <c r="P88" s="1"/>
-      <c r="S88" s="8"/>
-      <c r="T88" s="11"/>
-      <c r="U88" s="11"/>
-      <c r="V88" s="12"/>
+      <c r="L88" s="0"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="8"/>
+      <c r="R88" s="8"/>
+      <c r="S88" s="1"/>
+      <c r="V88" s="8"/>
+      <c r="W88" s="11"/>
+      <c r="X88" s="11"/>
+      <c r="Y88" s="12"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="7"/>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
-      <c r="M89" s="8"/>
-      <c r="O89" s="8"/>
-      <c r="P89" s="1"/>
-      <c r="S89" s="8"/>
-      <c r="T89" s="11"/>
-      <c r="U89" s="11"/>
-      <c r="V89" s="12"/>
+      <c r="L89" s="0"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="8"/>
+      <c r="R89" s="8"/>
+      <c r="S89" s="1"/>
+      <c r="V89" s="8"/>
+      <c r="W89" s="11"/>
+      <c r="X89" s="11"/>
+      <c r="Y89" s="12"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="7"/>
       <c r="J90" s="6"/>
       <c r="K90" s="6"/>
-      <c r="M90" s="8"/>
-      <c r="O90" s="8"/>
-      <c r="P90" s="1"/>
-      <c r="S90" s="8"/>
-      <c r="T90" s="11"/>
-      <c r="U90" s="11"/>
-      <c r="V90" s="12"/>
+      <c r="L90" s="0"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="8"/>
+      <c r="R90" s="8"/>
+      <c r="S90" s="1"/>
+      <c r="V90" s="8"/>
+      <c r="W90" s="11"/>
+      <c r="X90" s="11"/>
+      <c r="Y90" s="12"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="7"/>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
-      <c r="M91" s="8"/>
-      <c r="O91" s="8"/>
-      <c r="P91" s="1"/>
-      <c r="S91" s="8"/>
-      <c r="T91" s="11"/>
-      <c r="U91" s="11"/>
-      <c r="V91" s="12"/>
+      <c r="L91" s="0"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="8"/>
+      <c r="R91" s="8"/>
+      <c r="S91" s="1"/>
+      <c r="V91" s="8"/>
+      <c r="W91" s="11"/>
+      <c r="X91" s="11"/>
+      <c r="Y91" s="12"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="7"/>
       <c r="J92" s="6"/>
       <c r="K92" s="6"/>
-      <c r="M92" s="8"/>
-      <c r="O92" s="8"/>
-      <c r="P92" s="1"/>
-      <c r="S92" s="8"/>
-      <c r="T92" s="11"/>
-      <c r="U92" s="11"/>
-      <c r="V92" s="12"/>
+      <c r="L92" s="0"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="8"/>
+      <c r="R92" s="8"/>
+      <c r="S92" s="1"/>
+      <c r="V92" s="8"/>
+      <c r="W92" s="11"/>
+      <c r="X92" s="11"/>
+      <c r="Y92" s="12"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L93" s="0"/>
@@ -1562,58 +1761,285 @@
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L134" s="0"/>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L135" s="0"/>
+      <c r="O135" s="1"/>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L136" s="0"/>
+      <c r="O136" s="1"/>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L137" s="0"/>
+      <c r="O137" s="1"/>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L138" s="0"/>
+      <c r="O138" s="1"/>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L139" s="0"/>
+      <c r="O139" s="1"/>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L140" s="0"/>
+      <c r="O140" s="1"/>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L141" s="0"/>
+      <c r="O141" s="1"/>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L142" s="0"/>
+      <c r="O142" s="1"/>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L143" s="0"/>
+      <c r="O143" s="1"/>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L144" s="0"/>
+      <c r="O144" s="1"/>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L145" s="0"/>
+      <c r="O145" s="1"/>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L146" s="0"/>
+      <c r="O146" s="1"/>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L147" s="0"/>
+      <c r="O147" s="1"/>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L148" s="0"/>
+      <c r="O148" s="1"/>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L149" s="0"/>
+      <c r="O149" s="1"/>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L150" s="0"/>
+      <c r="O150" s="1"/>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L151" s="0"/>
+      <c r="O151" s="1"/>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L152" s="0"/>
+      <c r="O152" s="1"/>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L153" s="0"/>
+      <c r="O153" s="1"/>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L154" s="0"/>
+      <c r="O154" s="1"/>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L155" s="0"/>
+      <c r="O155" s="1"/>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L156" s="0"/>
+      <c r="O156" s="1"/>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L157" s="0"/>
+      <c r="O157" s="1"/>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L158" s="0"/>
+      <c r="O158" s="1"/>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L159" s="0"/>
+      <c r="O159" s="1"/>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L160" s="0"/>
+      <c r="O160" s="1"/>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L161" s="0"/>
+      <c r="O161" s="1"/>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L162" s="0"/>
+      <c r="O162" s="1"/>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L163" s="0"/>
+      <c r="O163" s="1"/>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L164" s="0"/>
+      <c r="O164" s="1"/>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L165" s="0"/>
+      <c r="O165" s="1"/>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L166" s="0"/>
+      <c r="O166" s="1"/>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L167" s="0"/>
+      <c r="O167" s="1"/>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L168" s="0"/>
+      <c r="O168" s="1"/>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L169" s="0"/>
+      <c r="O169" s="1"/>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L170" s="0"/>
+      <c r="O170" s="1"/>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L171" s="0"/>
+      <c r="O171" s="1"/>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L172" s="0"/>
+      <c r="O172" s="1"/>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L173" s="0"/>
+      <c r="O173" s="1"/>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L174" s="0"/>
+      <c r="O174" s="1"/>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L175" s="0"/>
+      <c r="O175" s="1"/>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L176" s="0"/>
+      <c r="O176" s="1"/>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L177" s="0"/>
+      <c r="O177" s="1"/>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L178" s="0"/>
+      <c r="O178" s="1"/>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L179" s="0"/>
+      <c r="O179" s="1"/>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L180" s="0"/>
+      <c r="O180" s="1"/>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L181" s="0"/>
+      <c r="O181" s="1"/>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L182" s="0"/>
+      <c r="O182" s="1"/>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L183" s="0"/>
+      <c r="O183" s="1"/>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L184" s="0"/>
+      <c r="O184" s="1"/>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L185" s="0"/>
+      <c r="O185" s="1"/>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L186" s="0"/>
+      <c r="O186" s="1"/>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L187" s="0"/>
+      <c r="O187" s="1"/>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L188" s="0"/>
+      <c r="O188" s="1"/>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L189" s="0"/>
+      <c r="O189" s="1"/>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L190" s="0"/>
+      <c r="O190" s="1"/>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L191" s="0"/>
+      <c r="O191" s="1"/>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L192" s="0"/>
+      <c r="O192" s="1"/>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L193" s="0"/>
+      <c r="O193" s="1"/>
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L194" s="0"/>
+      <c r="O194" s="1"/>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L195" s="0"/>
+      <c r="O195" s="1"/>
+    </row>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L196" s="0"/>
+      <c r="O196" s="1"/>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L197" s="0"/>
+      <c r="O197" s="1"/>
+    </row>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L198" s="0"/>
+      <c r="O198" s="1"/>
+    </row>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L199" s="0"/>
+      <c r="O199" s="1"/>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L200" s="0"/>
+      <c r="O200" s="1"/>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L201" s="0"/>
+      <c r="O201" s="1"/>
+    </row>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L202" s="0"/>
+      <c r="O202" s="1"/>
+    </row>
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L203" s="0"/>
+      <c r="O203" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:X134"/>
-  <mergeCells count="24">
+  <autoFilter ref="A1:AA68"/>
+  <mergeCells count="27">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1638,6 +2064,9 @@
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1655,17 +2084,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -1675,9 +2104,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.43"/>
@@ -1714,10 +2144,10 @@
       <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -1729,14 +2159,14 @@
       <c r="O1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>20</v>
@@ -1749,6 +2179,15 @@
       </c>
       <c r="V1" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1762,42 +2201,54 @@
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="P2" s="4"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="7"/>
       <c r="G3" s="8"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
     </row>
     <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="7"/>
       <c r="G4" s="8"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
     </row>
     <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="7"/>
       <c r="G5" s="8"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
     </row>
     <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7"/>
@@ -1805,13 +2256,16 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
+      <c r="O6" s="8"/>
       <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
     </row>
     <row r="7" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="7"/>
@@ -1819,13 +2273,16 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
       <c r="N7" s="8"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="8"/>
+      <c r="O7" s="8"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
     </row>
     <row r="8" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="7"/>
@@ -1833,13 +2290,16 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="8"/>
+      <c r="O8" s="8"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
     </row>
     <row r="9" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="7"/>
@@ -1847,13 +2307,16 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
       <c r="N9" s="8"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8"/>
+      <c r="O9" s="8"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
     </row>
     <row r="10" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="7"/>
@@ -1861,13 +2324,16 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
       <c r="N10" s="8"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="8"/>
+      <c r="O10" s="8"/>
       <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
     </row>
     <row r="11" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="7"/>
@@ -1875,13 +2341,16 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="8"/>
+      <c r="O11" s="8"/>
       <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
     </row>
     <row r="12" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="7"/>
@@ -1889,13 +2358,16 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
+      <c r="K12" s="0"/>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
       <c r="N12" s="8"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="8"/>
+      <c r="O12" s="8"/>
       <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
     </row>
     <row r="13" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="7"/>
@@ -1903,13 +2375,16 @@
       <c r="D13" s="14"/>
       <c r="E13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
       <c r="N13" s="8"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="8"/>
+      <c r="O13" s="8"/>
       <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
     </row>
     <row r="14" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="7"/>
@@ -2023,8 +2498,8 @@
       <c r="B35" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V19"/>
-  <mergeCells count="22">
+  <autoFilter ref="A1:Y13"/>
+  <mergeCells count="25">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -2047,6 +2522,9 @@
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2064,17 +2542,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T12" activeCellId="0" sqref="T12"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -2084,9 +2562,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.43"/>
@@ -2123,10 +2602,10 @@
       <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -2138,14 +2617,14 @@
       <c r="O1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>20</v>
@@ -2158,6 +2637,15 @@
       </c>
       <c r="V1" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2171,51 +2659,100 @@
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="P2" s="4"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="7"/>
       <c r="G3" s="8"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
     </row>
     <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
       <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
     </row>
     <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="7"/>
-      <c r="L5" s="8"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
     </row>
     <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7"/>
-      <c r="L6" s="8"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
     </row>
     <row r="7" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="7"/>
-      <c r="L7" s="8"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
     </row>
     <row r="8" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="7"/>
@@ -2223,13 +2760,16 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="8"/>
+      <c r="O8" s="8"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
     </row>
     <row r="9" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="7"/>
@@ -2237,13 +2777,16 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
       <c r="N9" s="8"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8"/>
+      <c r="O9" s="8"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
     </row>
     <row r="10" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="7"/>
@@ -2251,69 +2794,97 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
       <c r="N10" s="8"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="8"/>
+      <c r="O10" s="8"/>
       <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
     </row>
     <row r="11" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="8"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="N11" s="7"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
     </row>
     <row r="12" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
+      <c r="N12" s="0"/>
+      <c r="O12" s="0"/>
+      <c r="P12" s="0"/>
+      <c r="Q12" s="0"/>
+      <c r="R12" s="0"/>
+      <c r="S12" s="0"/>
+      <c r="T12" s="0"/>
+      <c r="U12" s="0"/>
+      <c r="V12" s="0"/>
     </row>
     <row r="13" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="N13" s="0"/>
+      <c r="O13" s="0"/>
+      <c r="P13" s="0"/>
+      <c r="Q13" s="0"/>
+      <c r="R13" s="0"/>
+      <c r="S13" s="0"/>
+      <c r="T13" s="0"/>
+      <c r="U13" s="0"/>
+      <c r="V13" s="0"/>
     </row>
     <row r="14" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
+      <c r="N14" s="0"/>
+      <c r="O14" s="0"/>
+      <c r="P14" s="0"/>
+      <c r="Q14" s="0"/>
+      <c r="R14" s="0"/>
+      <c r="S14" s="0"/>
+      <c r="T14" s="0"/>
+      <c r="U14" s="0"/>
+      <c r="V14" s="0"/>
     </row>
     <row r="15" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="7"/>
@@ -2384,18 +2955,36 @@
       <c r="V20" s="8"/>
     </row>
     <row r="21" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-    </row>
-    <row r="22" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
+      <c r="M21" s="0"/>
+      <c r="N21" s="0"/>
+      <c r="O21" s="0"/>
+      <c r="P21" s="0"/>
+      <c r="Q21" s="0"/>
+      <c r="R21" s="0"/>
+      <c r="S21" s="0"/>
+      <c r="T21" s="0"/>
+      <c r="U21" s="0"/>
+      <c r="V21" s="0"/>
+    </row>
+    <row r="22" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7"/>
       <c r="K22" s="7"/>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="7"/>
       <c r="K23" s="7"/>
       <c r="M23" s="8"/>
@@ -2474,8 +3063,8 @@
       <c r="B35" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V21"/>
-  <mergeCells count="23">
+  <autoFilter ref="A1:Y2"/>
+  <mergeCells count="26">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -2498,6 +3087,9 @@
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="B26:M26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2516,17 +3108,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -2537,9 +3129,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="29.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.43"/>
@@ -2576,10 +3169,10 @@
       <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -2591,14 +3184,14 @@
       <c r="O1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>20</v>
@@ -2611,6 +3204,15 @@
       </c>
       <c r="V1" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2624,26 +3226,32 @@
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="P2" s="4"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="7"/>
       <c r="G3" s="8"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
     </row>
     <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="7"/>
@@ -2651,12 +3259,15 @@
       <c r="D4" s="8"/>
       <c r="E4" s="17"/>
       <c r="G4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="8"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="8"/>
     </row>
     <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="7"/>
@@ -2664,12 +3275,15 @@
       <c r="D5" s="8"/>
       <c r="E5" s="17"/>
       <c r="G5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="8"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="8"/>
     </row>
     <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7"/>
@@ -2677,14 +3291,17 @@
       <c r="D6" s="8"/>
       <c r="E6" s="17"/>
       <c r="G6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="T6" s="18"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="W6" s="18"/>
     </row>
     <row r="7" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="7"/>
@@ -2692,13 +3309,16 @@
       <c r="D7" s="8"/>
       <c r="E7" s="17"/>
       <c r="G7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="17"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="T7" s="18"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="17"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="W7" s="18"/>
     </row>
     <row r="8" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="7"/>
@@ -2706,43 +3326,52 @@
       <c r="D8" s="8"/>
       <c r="E8" s="17"/>
       <c r="G8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="T8" s="18"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="W8" s="18"/>
     </row>
     <row r="9" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="7"/>
       <c r="G9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="T9" s="18"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="W9" s="18"/>
     </row>
     <row r="10" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="7"/>
       <c r="G10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="8"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="17"/>
       <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
+      <c r="U10" s="17"/>
       <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
     </row>
     <row r="11" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="7"/>
@@ -3037,8 +3666,8 @@
       <c r="M35" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V25"/>
-  <mergeCells count="22">
+  <autoFilter ref="A1:Y2"/>
+  <mergeCells count="25">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -3061,6 +3690,9 @@
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Update the sensor_table.xlsx and sensor_table_EXAMPLE.xlsx files and the gitlab_db_sensor.py script to be able to declare units for the uncertainty types
</commit_message>
<xml_diff>
--- a/sensor_table.xlsx
+++ b/sensor_table.xlsx
@@ -14,10 +14,14 @@
     <sheet name="Temperatur" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Druck!$A$1:$AB$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$Z$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$Z$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$Z$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Druck!$A$1:$AF$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$AD$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$AD$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$AD$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Druck!$A$1:$AB$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$Z$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$Z$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$Z$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="32">
   <si>
     <t xml:space="preserve">uuid</t>
   </si>
@@ -67,13 +71,25 @@
     <t xml:space="preserve">Sensitivity Uncertainty</t>
   </si>
   <si>
+    <t xml:space="preserve">Sensitivity Uncertainty Unit</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bias Uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bias Uncertainty Unit</t>
   </si>
   <si>
     <t xml:space="preserve">Linearity Uncertainty</t>
   </si>
   <si>
+    <t xml:space="preserve">Linearity Uncertainty Unit</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hysteresis Uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hysteresis Uncertainty Unit</t>
   </si>
   <si>
     <t xml:space="preserve">Messprinzip</t>
@@ -273,7 +289,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -334,6 +350,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,37 +382,6 @@
     <cellStyle name="Excel Built-in Neutral" xfId="21"/>
     <cellStyle name="Excel Built-in Note" xfId="22"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF232629"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFAC090"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCD5B5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -469,17 +466,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB203"/>
+  <dimension ref="A1:AF203"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AA3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
-      <selection pane="bottomRight" activeCell="A45" activeCellId="0" sqref="A45"/>
+      <selection pane="topRight" activeCell="AA1" activeCellId="0" sqref="AA1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -544,16 +541,16 @@
       <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="2" t="s">
@@ -562,7 +559,7 @@
       <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="2" t="s">
@@ -582,6 +579,18 @@
       </c>
       <c r="AB1" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -600,19 +609,23 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
-      <c r="S2" s="2"/>
+      <c r="S2" s="4"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
+      <c r="V2" s="4"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
@@ -2353,8 +2366,8 @@
       <c r="O203" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB2"/>
-  <mergeCells count="28">
+  <autoFilter ref="A1:AF2"/>
+  <mergeCells count="32">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -2383,10 +2396,14 @@
     <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AF1:AF2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2400,17 +2417,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z35"/>
+  <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="AC1" activeCellId="0" sqref="AC1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -2472,32 +2489,32 @@
       <c r="N1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>25</v>
@@ -2507,6 +2524,18 @@
       </c>
       <c r="Z1" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2524,18 +2553,22 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="2"/>
+      <c r="R2" s="4"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
+      <c r="U2" s="4"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
@@ -2957,8 +2990,8 @@
       <c r="B35" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z2"/>
-  <mergeCells count="26">
+  <autoFilter ref="A1:AD2"/>
+  <mergeCells count="30">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -2985,10 +3018,14 @@
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3002,17 +3039,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z35"/>
+  <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="Z1" activeCellId="0" sqref="Z1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -3074,32 +3111,32 @@
       <c r="N1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>25</v>
@@ -3109,6 +3146,18 @@
       </c>
       <c r="Z1" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3126,18 +3175,22 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="2"/>
+      <c r="R2" s="4"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
+      <c r="U2" s="4"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
@@ -3640,8 +3693,8 @@
       <c r="B35" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z2"/>
-  <mergeCells count="27">
+  <autoFilter ref="A1:AD2"/>
+  <mergeCells count="31">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -3668,11 +3721,15 @@
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="B26:M26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3686,17 +3743,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z35"/>
+  <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="Z1" activeCellId="0" sqref="Z1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="AD5" activeCellId="0" sqref="AD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -3714,6 +3771,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="20.46"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3759,32 +3821,32 @@
       <c r="N1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>25</v>
@@ -3794,6 +3856,18 @@
       </c>
       <c r="Z1" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3811,30 +3885,34 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="2"/>
+      <c r="R2" s="4"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
+      <c r="U2" s="4"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
@@ -3843,14 +3921,18 @@
       <c r="P3" s="0"/>
       <c r="Q3" s="0"/>
       <c r="R3" s="0"/>
-      <c r="S3" s="0"/>
-      <c r="T3" s="0"/>
-      <c r="U3" s="0"/>
-      <c r="V3" s="0"/>
-      <c r="W3" s="0"/>
-      <c r="X3" s="0"/>
-      <c r="Y3" s="0"/>
-      <c r="Z3" s="0"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
     </row>
     <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
@@ -4052,14 +4134,14 @@
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="15"/>
+      <c r="E11" s="18"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
+      <c r="L11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
@@ -4069,14 +4151,14 @@
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="18"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
+      <c r="L12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
@@ -4086,14 +4168,14 @@
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="15"/>
+      <c r="E13" s="18"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
+      <c r="L13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
@@ -4103,13 +4185,13 @@
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="15"/>
+      <c r="E14" s="18"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="15"/>
-      <c r="N14" s="15"/>
+      <c r="L14" s="18"/>
+      <c r="N14" s="18"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
@@ -4219,8 +4301,8 @@
     <row r="20" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7"/>
       <c r="K20" s="8"/>
-      <c r="L20" s="15"/>
-      <c r="N20" s="15"/>
+      <c r="L20" s="18"/>
+      <c r="N20" s="18"/>
       <c r="O20" s="7"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
@@ -4228,8 +4310,8 @@
     <row r="21" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="7"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="15"/>
-      <c r="N21" s="15"/>
+      <c r="L21" s="18"/>
+      <c r="N21" s="18"/>
       <c r="O21" s="7"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
@@ -4237,8 +4319,8 @@
     <row r="22" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="15"/>
-      <c r="N22" s="15"/>
+      <c r="L22" s="18"/>
+      <c r="N22" s="18"/>
       <c r="O22" s="7"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
@@ -4246,8 +4328,8 @@
     <row r="23" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="7"/>
       <c r="K23" s="8"/>
-      <c r="L23" s="15"/>
-      <c r="N23" s="15"/>
+      <c r="L23" s="18"/>
+      <c r="N23" s="18"/>
       <c r="O23" s="7"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
@@ -4341,8 +4423,8 @@
       <c r="M35" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z2"/>
-  <mergeCells count="26">
+  <autoFilter ref="A1:AD2"/>
+  <mergeCells count="30">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -4369,10 +4451,14 @@
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Add a 'Volumenstrom' sheet to the sensor tables
</commit_message>
<xml_diff>
--- a/sensor_table.xlsx
+++ b/sensor_table.xlsx
@@ -5,19 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Druck" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Kraft" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Weg" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Temperatur" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Volumenstrom" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Druck!$A$1:$AB$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$AI$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$AI$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$AI$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Druck!$A$1:$AO$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$AM$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$AM$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Volumenstrom!$A$1:$AM$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$AM$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="41">
   <si>
     <t xml:space="preserve">uuid</t>
   </si>
@@ -73,6 +75,9 @@
     <t xml:space="preserve">Sensitivity Uncertainty Comment</t>
   </si>
   <si>
+    <t xml:space="preserve">Sensitivity Uncertainty Keywords</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bias Uncertainty</t>
   </si>
   <si>
@@ -82,6 +87,9 @@
     <t xml:space="preserve">Bias Uncertainty Comment</t>
   </si>
   <si>
+    <t xml:space="preserve">Bias Uncertainty Keywords</t>
+  </si>
+  <si>
     <t xml:space="preserve">Linearity Uncertainty</t>
   </si>
   <si>
@@ -91,6 +99,9 @@
     <t xml:space="preserve">Linearity Uncertainty Comment</t>
   </si>
   <si>
+    <t xml:space="preserve">Linearity Uncertainty Keywords</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hysteresis Uncertainty</t>
   </si>
   <si>
@@ -98,6 +109,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hysteresis Uncertainty Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hysteresis Uncertainty Keywords</t>
   </si>
   <si>
     <t xml:space="preserve">Messprinzip</t>
@@ -300,7 +314,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -341,6 +355,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -349,11 +367,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -479,14 +497,18 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK203"/>
+  <dimension ref="A1:AO203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -494,25 +516,26 @@
       <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="7.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="115.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="105.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="39.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="23" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="42.57"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -585,16 +608,16 @@
       <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="2" t="s">
@@ -603,7 +626,7 @@
       <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
       </c>
       <c r="AE1" s="2" t="s">
@@ -626,6 +649,18 @@
       </c>
       <c r="AK1" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -652,13 +687,13 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
-      <c r="AA2" s="2"/>
+      <c r="AA2" s="4"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
+      <c r="AD2" s="4"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
@@ -666,598 +701,766 @@
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
-      <c r="AB3" s="1"/>
+      <c r="AF3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="AB4" s="1"/>
+      <c r="AF4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
-      <c r="AB5" s="1"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AF5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
-      <c r="AB6" s="1"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AF6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
-      <c r="AB7" s="1"/>
+      <c r="AF7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
-      <c r="AB8" s="1"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AF8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
-      <c r="AB9" s="1"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AF9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1"/>
-      <c r="AB10" s="1"/>
+      <c r="AF10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1"/>
-      <c r="AB11" s="1"/>
+      <c r="AF11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1"/>
-      <c r="AB12" s="1"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AF12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1"/>
-      <c r="AB13" s="1"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AF13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1"/>
-      <c r="AB14" s="1"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AF14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
-      <c r="AB15" s="1"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AF15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1"/>
-      <c r="AB16" s="1"/>
+      <c r="AF16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1"/>
-      <c r="AB17" s="1"/>
+      <c r="AF17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1"/>
-      <c r="AB18" s="1"/>
+      <c r="AF18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1"/>
-      <c r="AB19" s="1"/>
+      <c r="AF19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1"/>
-      <c r="AB20" s="1"/>
+      <c r="AF20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1"/>
-      <c r="AB21" s="1"/>
+      <c r="AF21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1"/>
-      <c r="AB22" s="1"/>
+      <c r="AF22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1"/>
-      <c r="AB23" s="1"/>
+      <c r="AF23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1"/>
-      <c r="AB24" s="1"/>
+      <c r="AF24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1"/>
-      <c r="AB25" s="1"/>
+      <c r="AF25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1"/>
-      <c r="AB26" s="1"/>
+      <c r="AF26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1"/>
-      <c r="AB27" s="1"/>
+      <c r="AF27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1"/>
-      <c r="AB28" s="1"/>
+      <c r="AF28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1"/>
-      <c r="AB29" s="1"/>
+      <c r="AF29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1"/>
-      <c r="AB30" s="1"/>
+      <c r="AF30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1"/>
-      <c r="AB31" s="1"/>
+      <c r="AF31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1"/>
-      <c r="AB32" s="1"/>
+      <c r="AF32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1"/>
-      <c r="AB33" s="1"/>
+      <c r="AF33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1"/>
-      <c r="AB34" s="1"/>
+      <c r="AF34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1"/>
-      <c r="AB35" s="1"/>
+      <c r="AF35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1"/>
-      <c r="AB36" s="1"/>
+      <c r="R36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
+      <c r="AF36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1"/>
-      <c r="AB37" s="1"/>
+      <c r="V37" s="5"/>
+      <c r="W37" s="5"/>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5"/>
+      <c r="AF37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1"/>
-      <c r="AB38" s="1"/>
+      <c r="V38" s="5"/>
+      <c r="W38" s="5"/>
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="5"/>
+      <c r="AF38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1"/>
-      <c r="AB39" s="1"/>
+      <c r="V39" s="5"/>
+      <c r="W39" s="5"/>
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="5"/>
+      <c r="AF39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="1"/>
-      <c r="AB40" s="1"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="5"/>
+      <c r="Z40" s="5"/>
+      <c r="AA40" s="5"/>
+      <c r="AF40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1"/>
-      <c r="AB41" s="1"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="5"/>
+      <c r="AF41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1"/>
-      <c r="AB42" s="1"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="5"/>
+      <c r="AF42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="1"/>
-      <c r="AB43" s="1"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="5"/>
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="5"/>
+      <c r="AF43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="1"/>
-      <c r="AB44" s="1"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="5"/>
+      <c r="AF44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="1"/>
-      <c r="AB45" s="1"/>
+      <c r="R45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="AF45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="1"/>
-      <c r="AB46" s="1"/>
+      <c r="R46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="AF46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="1"/>
-      <c r="AB47" s="1"/>
+      <c r="R47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="AF47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="1"/>
-      <c r="AB48" s="1"/>
+      <c r="R48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="AF48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="1"/>
-      <c r="AB49" s="1"/>
+      <c r="R49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="5"/>
+      <c r="AF49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="1"/>
-      <c r="AB50" s="1"/>
+      <c r="V50" s="5"/>
+      <c r="W50" s="5"/>
+      <c r="Z50" s="5"/>
+      <c r="AA50" s="5"/>
+      <c r="AF50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="1"/>
-      <c r="AB51" s="1"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="Z51" s="5"/>
+      <c r="AA51" s="5"/>
+      <c r="AF51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="1"/>
-      <c r="X52" s="1"/>
       <c r="AB52" s="1"/>
+      <c r="AF52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="1"/>
-      <c r="X53" s="1"/>
       <c r="AB53" s="1"/>
+      <c r="AF53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="1"/>
-      <c r="AB54" s="1"/>
+      <c r="AF54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="1"/>
-      <c r="AB55" s="1"/>
+      <c r="AF55" s="1"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="1"/>
-      <c r="AB56" s="1"/>
+      <c r="R56" s="5"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="5"/>
+      <c r="AF56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="1"/>
-      <c r="AB57" s="1"/>
+      <c r="R57" s="5"/>
+      <c r="V57" s="5"/>
+      <c r="W57" s="5"/>
+      <c r="AF57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="1"/>
-      <c r="AB58" s="1"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="Z58" s="5"/>
+      <c r="AA58" s="5"/>
+      <c r="AF58" s="1"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="1"/>
-      <c r="AB59" s="1"/>
+      <c r="V59" s="5"/>
+      <c r="W59" s="5"/>
+      <c r="Z59" s="5"/>
+      <c r="AA59" s="5"/>
+      <c r="AF59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="1"/>
-      <c r="AB60" s="1"/>
+      <c r="V60" s="5"/>
+      <c r="W60" s="5"/>
+      <c r="Z60" s="5"/>
+      <c r="AA60" s="5"/>
+      <c r="AF60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="1"/>
-      <c r="AB61" s="1"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="Z61" s="5"/>
+      <c r="AA61" s="5"/>
+      <c r="AF61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="1"/>
-      <c r="AB62" s="1"/>
+      <c r="R62" s="5"/>
+      <c r="V62" s="5"/>
+      <c r="W62" s="5"/>
+      <c r="AF62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="1"/>
-      <c r="AB63" s="1"/>
+      <c r="R63" s="5"/>
+      <c r="V63" s="5"/>
+      <c r="W63" s="5"/>
+      <c r="AF63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="1"/>
-      <c r="AB64" s="1"/>
+      <c r="AF64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="1"/>
-      <c r="X65" s="1"/>
+      <c r="R65" s="5"/>
+      <c r="V65" s="5"/>
+      <c r="W65" s="5"/>
+      <c r="AB65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="1"/>
-      <c r="X66" s="1"/>
+      <c r="R66" s="5"/>
+      <c r="V66" s="5"/>
+      <c r="W66" s="5"/>
+      <c r="AB66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="1"/>
-      <c r="X67" s="1"/>
+      <c r="R67" s="5"/>
+      <c r="V67" s="5"/>
+      <c r="W67" s="5"/>
+      <c r="AB67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="1"/>
-      <c r="X68" s="1"/>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R68" s="5"/>
+      <c r="V68" s="5"/>
+      <c r="W68" s="5"/>
+      <c r="AB68" s="1"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="S69" s="1"/>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P69" s="1"/>
+      <c r="U69" s="1"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="S70" s="1"/>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P70" s="1"/>
+      <c r="U70" s="1"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="S71" s="1"/>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P71" s="1"/>
+      <c r="U71" s="1"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="S72" s="1"/>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P72" s="1"/>
+      <c r="U72" s="1"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="S73" s="1"/>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P73" s="1"/>
+      <c r="U73" s="1"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="S74" s="1"/>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P74" s="1"/>
+      <c r="U74" s="1"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="S75" s="1"/>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P75" s="1"/>
+      <c r="U75" s="1"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1"/>
-      <c r="O76" s="1"/>
-      <c r="S76" s="6"/>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P76" s="1"/>
+      <c r="U76" s="6"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="S77" s="6"/>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P77" s="1"/>
+      <c r="U77" s="6"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1"/>
-      <c r="O78" s="1"/>
-      <c r="S78" s="6"/>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P78" s="1"/>
+      <c r="U78" s="6"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1"/>
-      <c r="O79" s="1"/>
-      <c r="S79" s="1"/>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P79" s="1"/>
+      <c r="U79" s="1"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="1"/>
-      <c r="O80" s="1"/>
-      <c r="S80" s="1"/>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P80" s="1"/>
+      <c r="U80" s="1"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="1"/>
-      <c r="O81" s="1"/>
-      <c r="S81" s="1"/>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P81" s="1"/>
+      <c r="U81" s="1"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="1"/>
-      <c r="O82" s="1"/>
-      <c r="S82" s="1"/>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P82" s="1"/>
+      <c r="U82" s="1"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="1"/>
-      <c r="O83" s="1"/>
-      <c r="S83" s="1"/>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P83" s="1"/>
+      <c r="U83" s="1"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="1"/>
-      <c r="O88" s="1"/>
-      <c r="S88" s="1"/>
-      <c r="W88" s="7"/>
-      <c r="X88" s="7"/>
-      <c r="Y88" s="8"/>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P88" s="1"/>
+      <c r="U88" s="1"/>
+      <c r="Z88" s="7"/>
+      <c r="AA88" s="7"/>
+      <c r="AB88" s="7"/>
+      <c r="AC88" s="8"/>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="1"/>
-      <c r="O89" s="1"/>
-      <c r="S89" s="1"/>
-      <c r="W89" s="7"/>
-      <c r="X89" s="7"/>
-      <c r="Y89" s="8"/>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P89" s="1"/>
+      <c r="U89" s="1"/>
+      <c r="Z89" s="7"/>
+      <c r="AA89" s="7"/>
+      <c r="AB89" s="7"/>
+      <c r="AC89" s="8"/>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="1"/>
-      <c r="O90" s="1"/>
-      <c r="S90" s="1"/>
-      <c r="W90" s="7"/>
-      <c r="X90" s="7"/>
-      <c r="Y90" s="8"/>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P90" s="1"/>
+      <c r="U90" s="1"/>
+      <c r="Z90" s="7"/>
+      <c r="AA90" s="7"/>
+      <c r="AB90" s="7"/>
+      <c r="AC90" s="8"/>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="1"/>
-      <c r="O91" s="1"/>
-      <c r="S91" s="1"/>
-      <c r="W91" s="7"/>
-      <c r="X91" s="7"/>
-      <c r="Y91" s="8"/>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P91" s="1"/>
+      <c r="U91" s="1"/>
+      <c r="Z91" s="7"/>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7"/>
+      <c r="AC91" s="8"/>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="1"/>
-      <c r="O92" s="1"/>
-      <c r="S92" s="1"/>
-      <c r="W92" s="7"/>
-      <c r="X92" s="7"/>
-      <c r="Y92" s="8"/>
-    </row>
+      <c r="P92" s="1"/>
+      <c r="U92" s="1"/>
+      <c r="Z92" s="7"/>
+      <c r="AA92" s="7"/>
+      <c r="AB92" s="7"/>
+      <c r="AC92" s="8"/>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O135" s="1"/>
+      <c r="P135" s="1"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O136" s="1"/>
+      <c r="P136" s="1"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O137" s="1"/>
+      <c r="P137" s="1"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O138" s="1"/>
+      <c r="P138" s="1"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O139" s="1"/>
+      <c r="P139" s="1"/>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O140" s="1"/>
+      <c r="P140" s="1"/>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O141" s="1"/>
+      <c r="P141" s="1"/>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O142" s="1"/>
+      <c r="P142" s="1"/>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O143" s="1"/>
+      <c r="P143" s="1"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O144" s="1"/>
+      <c r="P144" s="1"/>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O145" s="1"/>
+      <c r="P145" s="1"/>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O146" s="1"/>
+      <c r="P146" s="1"/>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O147" s="1"/>
+      <c r="P147" s="1"/>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O148" s="1"/>
+      <c r="P148" s="1"/>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O149" s="1"/>
+      <c r="P149" s="1"/>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O150" s="1"/>
+      <c r="P150" s="1"/>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O152" s="1"/>
+      <c r="P152" s="1"/>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O153" s="1"/>
+      <c r="P153" s="1"/>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O154" s="1"/>
+      <c r="P154" s="1"/>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O155" s="1"/>
+      <c r="P155" s="1"/>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O156" s="1"/>
+      <c r="P156" s="1"/>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O157" s="1"/>
+      <c r="P157" s="1"/>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O158" s="1"/>
+      <c r="P158" s="1"/>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O159" s="1"/>
+      <c r="P159" s="1"/>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O160" s="1"/>
+      <c r="P160" s="1"/>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O161" s="1"/>
+      <c r="P161" s="1"/>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O162" s="1"/>
+      <c r="P162" s="1"/>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O163" s="1"/>
+      <c r="P163" s="1"/>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O164" s="1"/>
+      <c r="P164" s="1"/>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O165" s="1"/>
+      <c r="P165" s="1"/>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O166" s="1"/>
+      <c r="P166" s="1"/>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O167" s="1"/>
+      <c r="P167" s="1"/>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O168" s="1"/>
+      <c r="P168" s="1"/>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O169" s="1"/>
+      <c r="P169" s="1"/>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O170" s="1"/>
+      <c r="P170" s="1"/>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O171" s="1"/>
+      <c r="P171" s="1"/>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O172" s="1"/>
+      <c r="P172" s="1"/>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O173" s="1"/>
+      <c r="P173" s="1"/>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O174" s="1"/>
+      <c r="P174" s="1"/>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O175" s="1"/>
+      <c r="P175" s="1"/>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O176" s="1"/>
+      <c r="P176" s="1"/>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O177" s="1"/>
+      <c r="P177" s="1"/>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O178" s="1"/>
+      <c r="P178" s="1"/>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O179" s="1"/>
+      <c r="P179" s="1"/>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O180" s="1"/>
+      <c r="P180" s="1"/>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O181" s="1"/>
+      <c r="P181" s="1"/>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O182" s="1"/>
+      <c r="P182" s="1"/>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O183" s="1"/>
+      <c r="P183" s="1"/>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O184" s="1"/>
+      <c r="P184" s="1"/>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O185" s="1"/>
+      <c r="P185" s="1"/>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O186" s="1"/>
+      <c r="P186" s="1"/>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O187" s="1"/>
+      <c r="P187" s="1"/>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O188" s="1"/>
+      <c r="P188" s="1"/>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O189" s="1"/>
+      <c r="P189" s="1"/>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O190" s="1"/>
+      <c r="P190" s="1"/>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O191" s="1"/>
+      <c r="P191" s="1"/>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O192" s="1"/>
+      <c r="P192" s="1"/>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O193" s="1"/>
+      <c r="P193" s="1"/>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O194" s="1"/>
+      <c r="P194" s="1"/>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O195" s="1"/>
+      <c r="P195" s="1"/>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O196" s="1"/>
+      <c r="P196" s="1"/>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O197" s="1"/>
+      <c r="P197" s="1"/>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O198" s="1"/>
+      <c r="P198" s="1"/>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O199" s="1"/>
+      <c r="P199" s="1"/>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O200" s="1"/>
+      <c r="P200" s="1"/>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O201" s="1"/>
+      <c r="P201" s="1"/>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O202" s="1"/>
+      <c r="P202" s="1"/>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O203" s="1"/>
+      <c r="P203" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB2"/>
-  <mergeCells count="37">
+  <autoFilter ref="A1:AO2"/>
+  <mergeCells count="41">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1295,6 +1498,10 @@
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="AJ1:AJ2"/>
     <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="AN1:AN2"/>
+    <mergeCell ref="AO1:AO2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1312,7 +1519,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI35"/>
+  <dimension ref="A1:AM35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -1322,27 +1529,27 @@
       <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="106.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="17" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="14.15"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1412,32 +1619,32 @@
       <c r="V1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>27</v>
       </c>
       <c r="AB1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="AF1" s="2" t="s">
         <v>33</v>
@@ -1450,6 +1657,18 @@
       </c>
       <c r="AI1" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1475,76 +1694,108 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
-      <c r="Z2" s="2"/>
+      <c r="Z2" s="4"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
+      <c r="AC2" s="4"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K3" s="0"/>
+      <c r="B3" s="1"/>
+      <c r="AE3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="0"/>
+      <c r="B4" s="1"/>
+      <c r="AE4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K5" s="0"/>
+      <c r="B5" s="1"/>
+      <c r="AE5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K6" s="0"/>
+      <c r="B6" s="1"/>
+      <c r="AE6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K7" s="0"/>
+      <c r="B7" s="1"/>
+      <c r="AE7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K8" s="0"/>
+      <c r="B8" s="1"/>
+      <c r="AE8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K9" s="0"/>
+      <c r="B9" s="1"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AE9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K10" s="0"/>
+      <c r="B10" s="1"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AE10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K11" s="0"/>
+      <c r="B11" s="1"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AE11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K12" s="0"/>
+      <c r="B12" s="1"/>
+      <c r="AE12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K13" s="0"/>
+      <c r="B13" s="1"/>
+      <c r="D13" s="10"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AE13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1"/>
-      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1"/>
@@ -1595,8 +1846,8 @@
       <c r="B35" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI2"/>
-  <mergeCells count="35">
+  <autoFilter ref="A1:AM2"/>
+  <mergeCells count="39">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1632,6 +1883,10 @@
     <mergeCell ref="AG1:AG2"/>
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1649,7 +1904,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI35"/>
+  <dimension ref="A1:AM35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -1659,28 +1914,29 @@
       <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="22.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="22.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="51.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="17.86"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1750,32 +2006,32 @@
       <c r="V1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>27</v>
       </c>
       <c r="AB1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="AF1" s="2" t="s">
         <v>33</v>
@@ -1788,6 +2044,18 @@
       </c>
       <c r="AI1" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1813,79 +2081,86 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
-      <c r="Z2" s="2"/>
+      <c r="Z2" s="4"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
+      <c r="AC2" s="4"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
-      <c r="AA3" s="1"/>
+      <c r="AE3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="AA4" s="1"/>
+      <c r="AE4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
-      <c r="AA5" s="1"/>
+      <c r="AE5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
-      <c r="AA6" s="1"/>
+      <c r="AE6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
-      <c r="AA7" s="1"/>
+      <c r="AE7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
-      <c r="AA8" s="1"/>
+      <c r="AE8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
-      <c r="AA9" s="1"/>
+      <c r="AE9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1"/>
-      <c r="AA10" s="1"/>
+      <c r="AE10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1"/>
-      <c r="W11" s="1"/>
-    </row>
+      <c r="AA11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1"/>
-      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1"/>
@@ -1899,19 +2174,20 @@
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
+    <row r="26" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1"/>
@@ -1941,8 +2217,8 @@
       <c r="B35" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI2"/>
-  <mergeCells count="36">
+  <autoFilter ref="A1:AM2"/>
+  <mergeCells count="39">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1978,7 +2254,10 @@
     <mergeCell ref="AG1:AG2"/>
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1996,39 +2275,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AI35"/>
+  <dimension ref="A1:AM35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="65.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="28.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="42.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="15.86"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2098,32 +2378,32 @@
       <c r="V1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>27</v>
       </c>
       <c r="AB1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="AF1" s="2" t="s">
         <v>33</v>
@@ -2136,6 +2416,18 @@
       </c>
       <c r="AI1" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2161,142 +2453,211 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
-      <c r="Z2" s="2"/>
+      <c r="Z2" s="4"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
+      <c r="AC2" s="4"/>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
-      <c r="AA3" s="1"/>
+      <c r="AE3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="E4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AB4" s="13"/>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
-      <c r="E5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AB5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
-      <c r="E6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="12"/>
-      <c r="AF6" s="8"/>
+      <c r="E6" s="13"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AB6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="13"/>
+      <c r="AJ6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
-      <c r="E7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="12"/>
-      <c r="AF7" s="8"/>
+      <c r="E7" s="13"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AB7" s="13"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="13"/>
+      <c r="AJ7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
-      <c r="E8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="12"/>
-      <c r="AF8" s="8"/>
+      <c r="E8" s="13"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AB8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="13"/>
+      <c r="AJ8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
-      <c r="X9" s="12"/>
-      <c r="Z9" s="12"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="12"/>
-      <c r="AF9" s="8"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AB9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="13"/>
+      <c r="AJ9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1"/>
-      <c r="X10" s="12"/>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="12"/>
-      <c r="AD10" s="12"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AB10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="13"/>
+      <c r="AH10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1"/>
-      <c r="E11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AB11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1"/>
-      <c r="E12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="N12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="L12" s="13"/>
       <c r="O12" s="13"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1"/>
-      <c r="E13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="N13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="L13" s="13"/>
       <c r="O13" s="13"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1"/>
-      <c r="E14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1"/>
-      <c r="L20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="1"/>
+      <c r="L20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1"/>
-      <c r="L21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="1"/>
+      <c r="L21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1"/>
-      <c r="L22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="1"/>
+      <c r="L22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1"/>
-      <c r="L23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="1"/>
+      <c r="L23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1"/>
@@ -2329,8 +2690,8 @@
       <c r="B35" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI2"/>
-  <mergeCells count="35">
+  <autoFilter ref="A1:AM2"/>
+  <mergeCells count="39">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -2366,6 +2727,10 @@
     <mergeCell ref="AG1:AG2"/>
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2376,4 +2741,252 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AM2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="0" width="22.92"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:AM2"/>
+  <mergeCells count="39">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>